<commit_message>
preparing for the webinar
</commit_message>
<xml_diff>
--- a/suppxls/Scen_Par-RPS_CO2p_GasP_Nuc.xlsx
+++ b/suppxls/Scen_Par-RPS_CO2p_GasP_Nuc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NewVEDA\Veda\Veda_models\Model_Demo_Adv_Veda\suppxls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\Model_Demo_Adv_Veda_Nov22\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372B172A-C4CE-4FC2-93F5-A4BDC0092FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3210319-52CA-43A9-9C23-73B26913B9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E4274E74-7A86-476E-8D8F-2DC29368AA80}"/>
+    <workbookView xWindow="3645" yWindow="3645" windowWidth="21600" windowHeight="12683" activeTab="1" xr2:uid="{E4274E74-7A86-476E-8D8F-2DC29368AA80}"/>
   </bookViews>
   <sheets>
     <sheet name="CaseDesc" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="52">
   <si>
     <t>Cset_CN</t>
   </si>
@@ -183,7 +183,22 @@
     <t>START</t>
   </si>
   <si>
-    <t>~InputCell: 1-8</t>
+    <t>~InputCell: 4,6,8</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>other_indexes</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>$ SET FIXBOH 2030</t>
+  </si>
+  <si>
+    <t>RFCmd_flags</t>
   </si>
 </sst>
 </file>
@@ -866,139 +881,139 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="2.5703125" customWidth="1"/>
-    <col min="259" max="259" width="111.140625" customWidth="1"/>
-    <col min="513" max="513" width="2.5703125" customWidth="1"/>
-    <col min="515" max="515" width="111.140625" customWidth="1"/>
-    <col min="769" max="769" width="2.5703125" customWidth="1"/>
-    <col min="771" max="771" width="111.140625" customWidth="1"/>
-    <col min="1025" max="1025" width="2.5703125" customWidth="1"/>
-    <col min="1027" max="1027" width="111.140625" customWidth="1"/>
-    <col min="1281" max="1281" width="2.5703125" customWidth="1"/>
-    <col min="1283" max="1283" width="111.140625" customWidth="1"/>
-    <col min="1537" max="1537" width="2.5703125" customWidth="1"/>
-    <col min="1539" max="1539" width="111.140625" customWidth="1"/>
-    <col min="1793" max="1793" width="2.5703125" customWidth="1"/>
-    <col min="1795" max="1795" width="111.140625" customWidth="1"/>
-    <col min="2049" max="2049" width="2.5703125" customWidth="1"/>
-    <col min="2051" max="2051" width="111.140625" customWidth="1"/>
-    <col min="2305" max="2305" width="2.5703125" customWidth="1"/>
-    <col min="2307" max="2307" width="111.140625" customWidth="1"/>
-    <col min="2561" max="2561" width="2.5703125" customWidth="1"/>
-    <col min="2563" max="2563" width="111.140625" customWidth="1"/>
-    <col min="2817" max="2817" width="2.5703125" customWidth="1"/>
-    <col min="2819" max="2819" width="111.140625" customWidth="1"/>
-    <col min="3073" max="3073" width="2.5703125" customWidth="1"/>
-    <col min="3075" max="3075" width="111.140625" customWidth="1"/>
-    <col min="3329" max="3329" width="2.5703125" customWidth="1"/>
-    <col min="3331" max="3331" width="111.140625" customWidth="1"/>
-    <col min="3585" max="3585" width="2.5703125" customWidth="1"/>
-    <col min="3587" max="3587" width="111.140625" customWidth="1"/>
-    <col min="3841" max="3841" width="2.5703125" customWidth="1"/>
-    <col min="3843" max="3843" width="111.140625" customWidth="1"/>
-    <col min="4097" max="4097" width="2.5703125" customWidth="1"/>
-    <col min="4099" max="4099" width="111.140625" customWidth="1"/>
-    <col min="4353" max="4353" width="2.5703125" customWidth="1"/>
-    <col min="4355" max="4355" width="111.140625" customWidth="1"/>
-    <col min="4609" max="4609" width="2.5703125" customWidth="1"/>
-    <col min="4611" max="4611" width="111.140625" customWidth="1"/>
-    <col min="4865" max="4865" width="2.5703125" customWidth="1"/>
-    <col min="4867" max="4867" width="111.140625" customWidth="1"/>
-    <col min="5121" max="5121" width="2.5703125" customWidth="1"/>
-    <col min="5123" max="5123" width="111.140625" customWidth="1"/>
-    <col min="5377" max="5377" width="2.5703125" customWidth="1"/>
-    <col min="5379" max="5379" width="111.140625" customWidth="1"/>
-    <col min="5633" max="5633" width="2.5703125" customWidth="1"/>
-    <col min="5635" max="5635" width="111.140625" customWidth="1"/>
-    <col min="5889" max="5889" width="2.5703125" customWidth="1"/>
-    <col min="5891" max="5891" width="111.140625" customWidth="1"/>
-    <col min="6145" max="6145" width="2.5703125" customWidth="1"/>
-    <col min="6147" max="6147" width="111.140625" customWidth="1"/>
-    <col min="6401" max="6401" width="2.5703125" customWidth="1"/>
-    <col min="6403" max="6403" width="111.140625" customWidth="1"/>
-    <col min="6657" max="6657" width="2.5703125" customWidth="1"/>
-    <col min="6659" max="6659" width="111.140625" customWidth="1"/>
-    <col min="6913" max="6913" width="2.5703125" customWidth="1"/>
-    <col min="6915" max="6915" width="111.140625" customWidth="1"/>
-    <col min="7169" max="7169" width="2.5703125" customWidth="1"/>
-    <col min="7171" max="7171" width="111.140625" customWidth="1"/>
-    <col min="7425" max="7425" width="2.5703125" customWidth="1"/>
-    <col min="7427" max="7427" width="111.140625" customWidth="1"/>
-    <col min="7681" max="7681" width="2.5703125" customWidth="1"/>
-    <col min="7683" max="7683" width="111.140625" customWidth="1"/>
-    <col min="7937" max="7937" width="2.5703125" customWidth="1"/>
-    <col min="7939" max="7939" width="111.140625" customWidth="1"/>
-    <col min="8193" max="8193" width="2.5703125" customWidth="1"/>
-    <col min="8195" max="8195" width="111.140625" customWidth="1"/>
-    <col min="8449" max="8449" width="2.5703125" customWidth="1"/>
-    <col min="8451" max="8451" width="111.140625" customWidth="1"/>
-    <col min="8705" max="8705" width="2.5703125" customWidth="1"/>
-    <col min="8707" max="8707" width="111.140625" customWidth="1"/>
-    <col min="8961" max="8961" width="2.5703125" customWidth="1"/>
-    <col min="8963" max="8963" width="111.140625" customWidth="1"/>
-    <col min="9217" max="9217" width="2.5703125" customWidth="1"/>
-    <col min="9219" max="9219" width="111.140625" customWidth="1"/>
-    <col min="9473" max="9473" width="2.5703125" customWidth="1"/>
-    <col min="9475" max="9475" width="111.140625" customWidth="1"/>
-    <col min="9729" max="9729" width="2.5703125" customWidth="1"/>
-    <col min="9731" max="9731" width="111.140625" customWidth="1"/>
-    <col min="9985" max="9985" width="2.5703125" customWidth="1"/>
-    <col min="9987" max="9987" width="111.140625" customWidth="1"/>
-    <col min="10241" max="10241" width="2.5703125" customWidth="1"/>
-    <col min="10243" max="10243" width="111.140625" customWidth="1"/>
-    <col min="10497" max="10497" width="2.5703125" customWidth="1"/>
-    <col min="10499" max="10499" width="111.140625" customWidth="1"/>
-    <col min="10753" max="10753" width="2.5703125" customWidth="1"/>
-    <col min="10755" max="10755" width="111.140625" customWidth="1"/>
-    <col min="11009" max="11009" width="2.5703125" customWidth="1"/>
-    <col min="11011" max="11011" width="111.140625" customWidth="1"/>
-    <col min="11265" max="11265" width="2.5703125" customWidth="1"/>
-    <col min="11267" max="11267" width="111.140625" customWidth="1"/>
-    <col min="11521" max="11521" width="2.5703125" customWidth="1"/>
-    <col min="11523" max="11523" width="111.140625" customWidth="1"/>
-    <col min="11777" max="11777" width="2.5703125" customWidth="1"/>
-    <col min="11779" max="11779" width="111.140625" customWidth="1"/>
-    <col min="12033" max="12033" width="2.5703125" customWidth="1"/>
-    <col min="12035" max="12035" width="111.140625" customWidth="1"/>
-    <col min="12289" max="12289" width="2.5703125" customWidth="1"/>
-    <col min="12291" max="12291" width="111.140625" customWidth="1"/>
-    <col min="12545" max="12545" width="2.5703125" customWidth="1"/>
-    <col min="12547" max="12547" width="111.140625" customWidth="1"/>
-    <col min="12801" max="12801" width="2.5703125" customWidth="1"/>
-    <col min="12803" max="12803" width="111.140625" customWidth="1"/>
-    <col min="13057" max="13057" width="2.5703125" customWidth="1"/>
-    <col min="13059" max="13059" width="111.140625" customWidth="1"/>
-    <col min="13313" max="13313" width="2.5703125" customWidth="1"/>
-    <col min="13315" max="13315" width="111.140625" customWidth="1"/>
-    <col min="13569" max="13569" width="2.5703125" customWidth="1"/>
-    <col min="13571" max="13571" width="111.140625" customWidth="1"/>
-    <col min="13825" max="13825" width="2.5703125" customWidth="1"/>
-    <col min="13827" max="13827" width="111.140625" customWidth="1"/>
-    <col min="14081" max="14081" width="2.5703125" customWidth="1"/>
-    <col min="14083" max="14083" width="111.140625" customWidth="1"/>
-    <col min="14337" max="14337" width="2.5703125" customWidth="1"/>
-    <col min="14339" max="14339" width="111.140625" customWidth="1"/>
-    <col min="14593" max="14593" width="2.5703125" customWidth="1"/>
-    <col min="14595" max="14595" width="111.140625" customWidth="1"/>
-    <col min="14849" max="14849" width="2.5703125" customWidth="1"/>
-    <col min="14851" max="14851" width="111.140625" customWidth="1"/>
-    <col min="15105" max="15105" width="2.5703125" customWidth="1"/>
-    <col min="15107" max="15107" width="111.140625" customWidth="1"/>
-    <col min="15361" max="15361" width="2.5703125" customWidth="1"/>
-    <col min="15363" max="15363" width="111.140625" customWidth="1"/>
-    <col min="15617" max="15617" width="2.5703125" customWidth="1"/>
-    <col min="15619" max="15619" width="111.140625" customWidth="1"/>
-    <col min="15873" max="15873" width="2.5703125" customWidth="1"/>
-    <col min="15875" max="15875" width="111.140625" customWidth="1"/>
-    <col min="16129" max="16129" width="2.5703125" customWidth="1"/>
-    <col min="16131" max="16131" width="111.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.59765625" customWidth="1"/>
+    <col min="3" max="3" width="32.73046875" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="2.59765625" customWidth="1"/>
+    <col min="259" max="259" width="111.1328125" customWidth="1"/>
+    <col min="513" max="513" width="2.59765625" customWidth="1"/>
+    <col min="515" max="515" width="111.1328125" customWidth="1"/>
+    <col min="769" max="769" width="2.59765625" customWidth="1"/>
+    <col min="771" max="771" width="111.1328125" customWidth="1"/>
+    <col min="1025" max="1025" width="2.59765625" customWidth="1"/>
+    <col min="1027" max="1027" width="111.1328125" customWidth="1"/>
+    <col min="1281" max="1281" width="2.59765625" customWidth="1"/>
+    <col min="1283" max="1283" width="111.1328125" customWidth="1"/>
+    <col min="1537" max="1537" width="2.59765625" customWidth="1"/>
+    <col min="1539" max="1539" width="111.1328125" customWidth="1"/>
+    <col min="1793" max="1793" width="2.59765625" customWidth="1"/>
+    <col min="1795" max="1795" width="111.1328125" customWidth="1"/>
+    <col min="2049" max="2049" width="2.59765625" customWidth="1"/>
+    <col min="2051" max="2051" width="111.1328125" customWidth="1"/>
+    <col min="2305" max="2305" width="2.59765625" customWidth="1"/>
+    <col min="2307" max="2307" width="111.1328125" customWidth="1"/>
+    <col min="2561" max="2561" width="2.59765625" customWidth="1"/>
+    <col min="2563" max="2563" width="111.1328125" customWidth="1"/>
+    <col min="2817" max="2817" width="2.59765625" customWidth="1"/>
+    <col min="2819" max="2819" width="111.1328125" customWidth="1"/>
+    <col min="3073" max="3073" width="2.59765625" customWidth="1"/>
+    <col min="3075" max="3075" width="111.1328125" customWidth="1"/>
+    <col min="3329" max="3329" width="2.59765625" customWidth="1"/>
+    <col min="3331" max="3331" width="111.1328125" customWidth="1"/>
+    <col min="3585" max="3585" width="2.59765625" customWidth="1"/>
+    <col min="3587" max="3587" width="111.1328125" customWidth="1"/>
+    <col min="3841" max="3841" width="2.59765625" customWidth="1"/>
+    <col min="3843" max="3843" width="111.1328125" customWidth="1"/>
+    <col min="4097" max="4097" width="2.59765625" customWidth="1"/>
+    <col min="4099" max="4099" width="111.1328125" customWidth="1"/>
+    <col min="4353" max="4353" width="2.59765625" customWidth="1"/>
+    <col min="4355" max="4355" width="111.1328125" customWidth="1"/>
+    <col min="4609" max="4609" width="2.59765625" customWidth="1"/>
+    <col min="4611" max="4611" width="111.1328125" customWidth="1"/>
+    <col min="4865" max="4865" width="2.59765625" customWidth="1"/>
+    <col min="4867" max="4867" width="111.1328125" customWidth="1"/>
+    <col min="5121" max="5121" width="2.59765625" customWidth="1"/>
+    <col min="5123" max="5123" width="111.1328125" customWidth="1"/>
+    <col min="5377" max="5377" width="2.59765625" customWidth="1"/>
+    <col min="5379" max="5379" width="111.1328125" customWidth="1"/>
+    <col min="5633" max="5633" width="2.59765625" customWidth="1"/>
+    <col min="5635" max="5635" width="111.1328125" customWidth="1"/>
+    <col min="5889" max="5889" width="2.59765625" customWidth="1"/>
+    <col min="5891" max="5891" width="111.1328125" customWidth="1"/>
+    <col min="6145" max="6145" width="2.59765625" customWidth="1"/>
+    <col min="6147" max="6147" width="111.1328125" customWidth="1"/>
+    <col min="6401" max="6401" width="2.59765625" customWidth="1"/>
+    <col min="6403" max="6403" width="111.1328125" customWidth="1"/>
+    <col min="6657" max="6657" width="2.59765625" customWidth="1"/>
+    <col min="6659" max="6659" width="111.1328125" customWidth="1"/>
+    <col min="6913" max="6913" width="2.59765625" customWidth="1"/>
+    <col min="6915" max="6915" width="111.1328125" customWidth="1"/>
+    <col min="7169" max="7169" width="2.59765625" customWidth="1"/>
+    <col min="7171" max="7171" width="111.1328125" customWidth="1"/>
+    <col min="7425" max="7425" width="2.59765625" customWidth="1"/>
+    <col min="7427" max="7427" width="111.1328125" customWidth="1"/>
+    <col min="7681" max="7681" width="2.59765625" customWidth="1"/>
+    <col min="7683" max="7683" width="111.1328125" customWidth="1"/>
+    <col min="7937" max="7937" width="2.59765625" customWidth="1"/>
+    <col min="7939" max="7939" width="111.1328125" customWidth="1"/>
+    <col min="8193" max="8193" width="2.59765625" customWidth="1"/>
+    <col min="8195" max="8195" width="111.1328125" customWidth="1"/>
+    <col min="8449" max="8449" width="2.59765625" customWidth="1"/>
+    <col min="8451" max="8451" width="111.1328125" customWidth="1"/>
+    <col min="8705" max="8705" width="2.59765625" customWidth="1"/>
+    <col min="8707" max="8707" width="111.1328125" customWidth="1"/>
+    <col min="8961" max="8961" width="2.59765625" customWidth="1"/>
+    <col min="8963" max="8963" width="111.1328125" customWidth="1"/>
+    <col min="9217" max="9217" width="2.59765625" customWidth="1"/>
+    <col min="9219" max="9219" width="111.1328125" customWidth="1"/>
+    <col min="9473" max="9473" width="2.59765625" customWidth="1"/>
+    <col min="9475" max="9475" width="111.1328125" customWidth="1"/>
+    <col min="9729" max="9729" width="2.59765625" customWidth="1"/>
+    <col min="9731" max="9731" width="111.1328125" customWidth="1"/>
+    <col min="9985" max="9985" width="2.59765625" customWidth="1"/>
+    <col min="9987" max="9987" width="111.1328125" customWidth="1"/>
+    <col min="10241" max="10241" width="2.59765625" customWidth="1"/>
+    <col min="10243" max="10243" width="111.1328125" customWidth="1"/>
+    <col min="10497" max="10497" width="2.59765625" customWidth="1"/>
+    <col min="10499" max="10499" width="111.1328125" customWidth="1"/>
+    <col min="10753" max="10753" width="2.59765625" customWidth="1"/>
+    <col min="10755" max="10755" width="111.1328125" customWidth="1"/>
+    <col min="11009" max="11009" width="2.59765625" customWidth="1"/>
+    <col min="11011" max="11011" width="111.1328125" customWidth="1"/>
+    <col min="11265" max="11265" width="2.59765625" customWidth="1"/>
+    <col min="11267" max="11267" width="111.1328125" customWidth="1"/>
+    <col min="11521" max="11521" width="2.59765625" customWidth="1"/>
+    <col min="11523" max="11523" width="111.1328125" customWidth="1"/>
+    <col min="11777" max="11777" width="2.59765625" customWidth="1"/>
+    <col min="11779" max="11779" width="111.1328125" customWidth="1"/>
+    <col min="12033" max="12033" width="2.59765625" customWidth="1"/>
+    <col min="12035" max="12035" width="111.1328125" customWidth="1"/>
+    <col min="12289" max="12289" width="2.59765625" customWidth="1"/>
+    <col min="12291" max="12291" width="111.1328125" customWidth="1"/>
+    <col min="12545" max="12545" width="2.59765625" customWidth="1"/>
+    <col min="12547" max="12547" width="111.1328125" customWidth="1"/>
+    <col min="12801" max="12801" width="2.59765625" customWidth="1"/>
+    <col min="12803" max="12803" width="111.1328125" customWidth="1"/>
+    <col min="13057" max="13057" width="2.59765625" customWidth="1"/>
+    <col min="13059" max="13059" width="111.1328125" customWidth="1"/>
+    <col min="13313" max="13313" width="2.59765625" customWidth="1"/>
+    <col min="13315" max="13315" width="111.1328125" customWidth="1"/>
+    <col min="13569" max="13569" width="2.59765625" customWidth="1"/>
+    <col min="13571" max="13571" width="111.1328125" customWidth="1"/>
+    <col min="13825" max="13825" width="2.59765625" customWidth="1"/>
+    <col min="13827" max="13827" width="111.1328125" customWidth="1"/>
+    <col min="14081" max="14081" width="2.59765625" customWidth="1"/>
+    <col min="14083" max="14083" width="111.1328125" customWidth="1"/>
+    <col min="14337" max="14337" width="2.59765625" customWidth="1"/>
+    <col min="14339" max="14339" width="111.1328125" customWidth="1"/>
+    <col min="14593" max="14593" width="2.59765625" customWidth="1"/>
+    <col min="14595" max="14595" width="111.1328125" customWidth="1"/>
+    <col min="14849" max="14849" width="2.59765625" customWidth="1"/>
+    <col min="14851" max="14851" width="111.1328125" customWidth="1"/>
+    <col min="15105" max="15105" width="2.59765625" customWidth="1"/>
+    <col min="15107" max="15107" width="111.1328125" customWidth="1"/>
+    <col min="15361" max="15361" width="2.59765625" customWidth="1"/>
+    <col min="15363" max="15363" width="111.1328125" customWidth="1"/>
+    <col min="15617" max="15617" width="2.59765625" customWidth="1"/>
+    <col min="15619" max="15619" width="111.1328125" customWidth="1"/>
+    <col min="15873" max="15873" width="2.59765625" customWidth="1"/>
+    <col min="15875" max="15875" width="111.1328125" customWidth="1"/>
+    <col min="16129" max="16129" width="2.59765625" customWidth="1"/>
+    <col min="16131" max="16131" width="111.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:22" x14ac:dyDescent="0.45">
       <c r="D1" s="34" t="s">
         <v>5</v>
       </c>
@@ -1021,7 +1036,7 @@
       <c r="U1" s="34"/>
       <c r="V1" s="34"/>
     </row>
-    <row r="2" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1029,7 +1044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:22" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -1038,7 +1053,7 @@
         <v>RPS-0.CO2p-0.05.GasP-1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -1047,7 +1062,7 @@
         <v>RPS-0.CO2p-0.1.GasP-1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B5" s="4">
         <f>B4+1</f>
         <v>3</v>
@@ -1057,7 +1072,7 @@
         <v>RPS-0.CO2p-0.15.GasP-1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B6" s="4">
         <f t="shared" ref="B6:B69" si="0">B5+1</f>
         <v>4</v>
@@ -1067,7 +1082,7 @@
         <v>RPS-0.CO2p-0.2.GasP-1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B7" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1077,7 +1092,7 @@
         <v>RPS-0.CO2p-0.25.GasP-1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B8" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1087,7 +1102,7 @@
         <v>RPS-0.CO2p-0.3.GasP-1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B9" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1097,7 +1112,7 @@
         <v>RPS-0.CO2p-0.35.GasP-1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B10" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1107,7 +1122,7 @@
         <v>RPS-0.CO2p-0.4.GasP-1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B11" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1117,7 +1132,7 @@
         <v>RPS-0.CO2p-0.2.GasP-1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B12" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1127,7 +1142,7 @@
         <v>RPS-0.CO2p-0.2.GasP-1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B13" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1137,7 +1152,7 @@
         <v>RPS-0.CO2p-0.2.GasP-1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B14" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1147,7 +1162,7 @@
         <v>RPS-0.CO2p-0.2.GasP-1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B15" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1157,7 +1172,7 @@
         <v>RPS-0.CO2p-0.05.GasP-0.9.Nuc-Y.</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B16" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1167,7 +1182,7 @@
         <v>RPS-0.CO2p-0.1.GasP-0.9.Nuc-Y.</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B17" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1177,7 +1192,7 @@
         <v>RPS-0.CO2p-0.15.GasP-0.9.Nuc-Y.</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B18" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1187,7 +1202,7 @@
         <v>RPS-0.CO2p-0.2.GasP-0.9.Nuc-Y.</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B19" s="4">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1197,7 +1212,7 @@
         <v>RPS-0.CO2p-0.25.GasP-0.9.Nuc-Y.</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1207,7 +1222,7 @@
         <v>RPS-0.CO2p-0.3.GasP-0.9.Nuc-Y.</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B21" s="4">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1217,7 +1232,7 @@
         <v>RPS-0.CO2p-0.35.GasP-0.9.Nuc-Y.</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B22" s="4">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1227,7 +1242,7 @@
         <v>RPS-0.CO2p-0.4.GasP-0.9.Nuc-Y.</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B23" s="4">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1237,7 +1252,7 @@
         <v>RPS-0.CO2p-0.2.GasP-0.9.Nuc-Y.</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B24" s="4">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1247,7 +1262,7 @@
         <v>RPS-0.CO2p-0.2.GasP-0.9.Nuc-Y.</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B25" s="4">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1257,7 +1272,7 @@
         <v>RPS-0.CO2p-0.2.GasP-0.9.Nuc-Y.</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B26" s="4">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1267,7 +1282,7 @@
         <v>RPS-0.CO2p-0.2.GasP-0.9.Nuc-Y.</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B27" s="4">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1277,7 +1292,7 @@
         <v>RPS-0.CO2p-0.05.GasP-1.1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B28" s="4">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1287,7 +1302,7 @@
         <v>RPS-0.CO2p-0.1.GasP-1.1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B29" s="4">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1297,7 +1312,7 @@
         <v>RPS-0.CO2p-0.15.GasP-1.1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B30" s="4">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1307,7 +1322,7 @@
         <v>RPS-0.CO2p-0.2.GasP-1.1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B31" s="4">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1317,7 +1332,7 @@
         <v>RPS-0.CO2p-0.25.GasP-1.1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B32" s="4">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1327,7 +1342,7 @@
         <v>RPS-0.CO2p-0.3.GasP-1.1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B33" s="4">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1337,7 +1352,7 @@
         <v>RPS-0.CO2p-0.35.GasP-1.1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B34" s="4">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1347,7 +1362,7 @@
         <v>RPS-0.CO2p-0.4.GasP-1.1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B35" s="4">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1357,7 +1372,7 @@
         <v>RPS-0.CO2p-0.2.GasP-1.1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B36" s="4">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1367,7 +1382,7 @@
         <v>RPS-0.CO2p-0.2.GasP-1.1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B37" s="4">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1377,7 +1392,7 @@
         <v>RPS-0.CO2p-0.2.GasP-1.1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B38" s="4">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1387,7 +1402,7 @@
         <v>RPS-0.CO2p-0.2.GasP-1.1.Nuc-Y.</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B39" s="4">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1397,7 +1412,7 @@
         <v>RPS-0.CO2p-0.05.GasP-1.Nuc-N.</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B40" s="4">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1407,7 +1422,7 @@
         <v>RPS-0.CO2p-0.1.GasP-1.Nuc-N.</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B41" s="4">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1417,7 +1432,7 @@
         <v>RPS-0.CO2p-0.15.GasP-1.Nuc-N.</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B42" s="4">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1427,7 +1442,7 @@
         <v>RPS-0.CO2p-0.2.GasP-1.Nuc-N.</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B43" s="4">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1437,7 +1452,7 @@
         <v>RPS-0.CO2p-0.25.GasP-1.Nuc-N.</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B44" s="4">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1447,7 +1462,7 @@
         <v>RPS-0.CO2p-0.3.GasP-1.Nuc-N.</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B45" s="4">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1457,7 +1472,7 @@
         <v>RPS-0.CO2p-0.35.GasP-1.Nuc-N.</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B46" s="4">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1467,7 +1482,7 @@
         <v>RPS-0.CO2p-0.4.GasP-1.Nuc-N.</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B47" s="4">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1477,7 +1492,7 @@
         <v>RPS-0.CO2p-0.2.GasP-1.Nuc-N.</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B48" s="4">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1487,7 +1502,7 @@
         <v>RPS-0.CO2p-0.2.GasP-1.Nuc-N.</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B49" s="4">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1497,7 +1512,7 @@
         <v>RPS-0.CO2p-0.2.GasP-1.Nuc-N.</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B50" s="4">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -1507,7 +1522,7 @@
         <v>RPS-0.CO2p-0.2.GasP-1.Nuc-N.</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B51" s="4">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -1517,7 +1532,7 @@
         <v>RPS-0.CO2p-0.05.GasP-0.9.Nuc-N.</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B52" s="4">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -1527,7 +1542,7 @@
         <v>RPS-0.CO2p-0.1.GasP-0.9.Nuc-N.</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B53" s="4">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -1537,7 +1552,7 @@
         <v>RPS-0.CO2p-0.15.GasP-0.9.Nuc-N.</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B54" s="4">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -1547,7 +1562,7 @@
         <v>RPS-0.CO2p-0.2.GasP-0.9.Nuc-N.</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B55" s="4">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -1557,7 +1572,7 @@
         <v>RPS-0.CO2p-0.25.GasP-0.9.Nuc-N.</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B56" s="4">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -1567,7 +1582,7 @@
         <v>RPS-0.CO2p-0.3.GasP-0.9.Nuc-N.</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B57" s="4">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -1577,7 +1592,7 @@
         <v>RPS-0.CO2p-0.35.GasP-0.9.Nuc-N.</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B58" s="4">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -1587,7 +1602,7 @@
         <v>RPS-0.CO2p-0.4.GasP-0.9.Nuc-N.</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B59" s="4">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -1597,7 +1612,7 @@
         <v>RPS-0.CO2p-0.2.GasP-0.9.Nuc-N.</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B60" s="4">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -1607,7 +1622,7 @@
         <v>RPS-0.CO2p-0.2.GasP-0.9.Nuc-N.</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B61" s="4">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -1617,7 +1632,7 @@
         <v>RPS-0.CO2p-0.2.GasP-0.9.Nuc-N.</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B62" s="4">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -1627,7 +1642,7 @@
         <v>RPS-0.CO2p-0.2.GasP-0.9.Nuc-N.</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B63" s="4">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -1637,7 +1652,7 @@
         <v>RPS-0.CO2p-0.05.GasP-1.1.Nuc-N.</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B64" s="4">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -1647,7 +1662,7 @@
         <v>RPS-0.CO2p-0.1.GasP-1.1.Nuc-N.</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B65" s="4">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -1657,7 +1672,7 @@
         <v>RPS-0.CO2p-0.15.GasP-1.1.Nuc-N.</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B66" s="4">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -1667,7 +1682,7 @@
         <v>RPS-0.CO2p-0.2.GasP-1.1.Nuc-N.</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B67" s="4">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -1677,7 +1692,7 @@
         <v>RPS-0.CO2p-0.25.GasP-1.1.Nuc-N.</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B68" s="4">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -1687,7 +1702,7 @@
         <v>RPS-0.CO2p-0.3.GasP-1.1.Nuc-N.</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B69" s="4">
         <f t="shared" si="0"/>
         <v>67</v>
@@ -1697,7 +1712,7 @@
         <v>RPS-0.CO2p-0.35.GasP-1.1.Nuc-N.</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B70" s="4">
         <f t="shared" ref="B70:B74" si="1">B69+1</f>
         <v>68</v>
@@ -1707,7 +1722,7 @@
         <v>RPS-0.CO2p-0.4.GasP-1.1.Nuc-N.</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B71" s="4">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -1717,7 +1732,7 @@
         <v>RPS-0.CO2p-0.2.GasP-1.1.Nuc-N.</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B72" s="4">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -1727,7 +1742,7 @@
         <v>RPS-0.CO2p-0.2.GasP-1.1.Nuc-N.</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B73" s="4">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -1737,7 +1752,7 @@
         <v>RPS-0.CO2p-0.2.GasP-1.1.Nuc-N.</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B74" s="4">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -1761,38 +1776,61 @@
   <dimension ref="A1:AA79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="8.140625" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="8.1328125" customWidth="1"/>
+    <col min="7" max="7" width="8.86328125" customWidth="1"/>
+    <col min="8" max="8" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.59765625" customWidth="1"/>
+    <col min="10" max="10" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.1328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.1328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="L3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" t="s">
+        <v>50</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
       <c r="C5" s="11">
         <f>VLOOKUP($A$2,$B$8:$F$198,C6,FALSE)</f>
         <v>0</v>
@@ -1813,7 +1851,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="C6" s="12">
         <v>2</v>
       </c>
@@ -1842,7 +1880,7 @@
       <c r="S6" s="26"/>
       <c r="T6" s="26"/>
     </row>
-    <row r="7" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B7" s="13" t="s">
         <v>4</v>
       </c>
@@ -1870,7 +1908,7 @@
       <c r="Z7" s="24"/>
       <c r="AA7" s="24"/>
     </row>
-    <row r="8" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B8" s="13">
         <v>1</v>
       </c>
@@ -1937,7 +1975,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B9" s="13">
         <v>2</v>
       </c>
@@ -2007,7 +2045,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B10" s="13">
         <v>3</v>
       </c>
@@ -2041,7 +2079,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B11" s="13">
         <v>4</v>
       </c>
@@ -2075,7 +2113,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B12" s="13">
         <v>5</v>
       </c>
@@ -2109,7 +2147,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B13" s="13">
         <v>6</v>
       </c>
@@ -2157,7 +2195,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B14" s="13">
         <v>7</v>
       </c>
@@ -2195,7 +2233,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="13">
         <v>8</v>
       </c>
@@ -2250,7 +2288,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B16" s="13">
         <v>9</v>
       </c>
@@ -2297,7 +2335,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="17" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B17" s="13">
         <v>10</v>
       </c>
@@ -2346,7 +2384,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="18" spans="2:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:27" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="13">
         <v>11</v>
       </c>
@@ -2397,7 +2435,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="19" spans="2:27" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:27" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B19" s="13">
         <v>12</v>
       </c>
@@ -2446,7 +2484,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="20" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B20" s="13">
         <v>13</v>
       </c>
@@ -2481,7 +2519,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="21" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B21" s="13">
         <v>14</v>
       </c>
@@ -2516,7 +2554,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="22" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B22" s="13">
         <v>15</v>
       </c>
@@ -2565,7 +2603,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="23" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B23" s="13">
         <v>16</v>
       </c>
@@ -2605,7 +2643,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="24" spans="2:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:27" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="13">
         <v>17</v>
       </c>
@@ -2664,7 +2702,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="25" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B25" s="13">
         <v>18</v>
       </c>
@@ -2713,7 +2751,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="26" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B26" s="13">
         <v>19</v>
       </c>
@@ -2748,7 +2786,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="27" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B27" s="13">
         <v>20</v>
       </c>
@@ -2783,7 +2821,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="28" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B28" s="13">
         <v>21</v>
       </c>
@@ -2818,7 +2856,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="29" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:27" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B29" s="13">
         <v>22</v>
       </c>
@@ -2867,7 +2905,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="30" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B30" s="13">
         <v>23</v>
       </c>
@@ -2905,7 +2943,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="31" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:27" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B31" s="13">
         <v>24</v>
       </c>
@@ -2954,7 +2992,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="32" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B32" s="13">
         <v>25</v>
       </c>
@@ -2997,7 +3035,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="33" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B33" s="13">
         <v>26</v>
       </c>
@@ -3031,7 +3069,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="34" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B34" s="13">
         <v>27</v>
       </c>
@@ -3065,7 +3103,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="35" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B35" s="13">
         <v>28</v>
       </c>
@@ -3099,7 +3137,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="36" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B36" s="13">
         <v>29</v>
       </c>
@@ -3133,7 +3171,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="37" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B37" s="13">
         <v>30</v>
       </c>
@@ -3167,7 +3205,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="38" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B38" s="13">
         <v>31</v>
       </c>
@@ -3201,7 +3239,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="39" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B39" s="13">
         <v>32</v>
       </c>
@@ -3235,7 +3273,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="40" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B40" s="13">
         <v>33</v>
       </c>
@@ -3269,7 +3307,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="41" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B41" s="13">
         <v>34</v>
       </c>
@@ -3303,7 +3341,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="42" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B42" s="13">
         <v>35</v>
       </c>
@@ -3337,7 +3375,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="43" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B43" s="13">
         <v>36</v>
       </c>
@@ -3371,7 +3409,7 @@
         <v>Nuc-Y.</v>
       </c>
     </row>
-    <row r="44" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B44" s="13">
         <v>37</v>
       </c>
@@ -3406,7 +3444,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="45" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B45" s="13">
         <v>38</v>
       </c>
@@ -3441,7 +3479,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="46" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B46" s="13">
         <v>39</v>
       </c>
@@ -3476,7 +3514,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="47" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B47" s="13">
         <v>40</v>
       </c>
@@ -3511,7 +3549,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="48" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B48" s="13">
         <v>41</v>
       </c>
@@ -3546,7 +3584,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="49" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B49" s="13">
         <v>42</v>
       </c>
@@ -3581,7 +3619,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="50" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B50" s="13">
         <v>43</v>
       </c>
@@ -3616,7 +3654,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="51" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B51" s="13">
         <v>44</v>
       </c>
@@ -3651,7 +3689,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="52" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B52" s="13">
         <v>45</v>
       </c>
@@ -3686,7 +3724,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="53" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B53" s="13">
         <v>46</v>
       </c>
@@ -3721,7 +3759,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="54" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B54" s="13">
         <v>47</v>
       </c>
@@ -3756,7 +3794,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="55" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B55" s="13">
         <v>48</v>
       </c>
@@ -3791,7 +3829,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="56" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B56" s="13">
         <v>49</v>
       </c>
@@ -3826,7 +3864,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="57" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B57" s="13">
         <v>50</v>
       </c>
@@ -3861,7 +3899,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="58" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B58" s="13">
         <v>51</v>
       </c>
@@ -3896,7 +3934,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="59" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B59" s="13">
         <v>52</v>
       </c>
@@ -3931,7 +3969,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="60" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B60" s="13">
         <v>53</v>
       </c>
@@ -3966,7 +4004,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="61" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B61" s="13">
         <v>54</v>
       </c>
@@ -4001,7 +4039,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="62" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B62" s="13">
         <v>55</v>
       </c>
@@ -4036,7 +4074,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="63" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B63" s="13">
         <v>56</v>
       </c>
@@ -4071,7 +4109,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="64" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B64" s="13">
         <v>57</v>
       </c>
@@ -4106,7 +4144,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="65" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B65" s="13">
         <v>58</v>
       </c>
@@ -4141,7 +4179,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="66" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B66" s="13">
         <v>59</v>
       </c>
@@ -4176,7 +4214,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="67" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B67" s="13">
         <v>60</v>
       </c>
@@ -4211,7 +4249,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="68" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B68" s="13">
         <v>61</v>
       </c>
@@ -4246,7 +4284,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="69" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B69" s="13">
         <v>62</v>
       </c>
@@ -4281,7 +4319,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="70" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B70" s="13">
         <v>63</v>
       </c>
@@ -4316,7 +4354,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="71" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B71" s="13">
         <v>64</v>
       </c>
@@ -4351,7 +4389,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="72" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B72" s="13">
         <v>65</v>
       </c>
@@ -4386,7 +4424,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="73" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B73" s="13">
         <v>66</v>
       </c>
@@ -4421,7 +4459,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="74" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B74" s="13">
         <v>67</v>
       </c>
@@ -4456,7 +4494,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="75" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B75" s="13">
         <v>68</v>
       </c>
@@ -4491,7 +4529,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="76" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B76" s="13">
         <v>69</v>
       </c>
@@ -4526,7 +4564,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="77" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B77" s="13">
         <v>70</v>
       </c>
@@ -4561,7 +4599,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="78" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B78" s="13">
         <v>71</v>
       </c>
@@ -4596,7 +4634,7 @@
         <v>Nuc-N.</v>
       </c>
     </row>
-    <row r="79" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B79" s="13">
         <v>72</v>
       </c>
@@ -4644,12 +4682,12 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>1</v>
       </c>
@@ -4658,7 +4696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>2</v>
       </c>
@@ -4667,7 +4705,7 @@
         <v>1,2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>3</v>
       </c>
@@ -4676,7 +4714,7 @@
         <v>1,2,3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>4</v>
       </c>
@@ -4685,7 +4723,7 @@
         <v>1,2,3,4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>13</v>
       </c>
@@ -4694,7 +4732,7 @@
         <v>1,2,3,4,13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>14</v>
       </c>
@@ -4703,7 +4741,7 @@
         <v>1,2,3,4,13,14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>15</v>
       </c>
@@ -4712,7 +4750,7 @@
         <v>1,2,3,4,13,14,15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>16</v>
       </c>
@@ -4721,7 +4759,7 @@
         <v>1,2,3,4,13,14,15,16</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>25</v>
       </c>
@@ -4730,7 +4768,7 @@
         <v>1,2,3,4,13,14,15,16,25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>26</v>
       </c>
@@ -4739,7 +4777,7 @@
         <v>1,2,3,4,13,14,15,16,25,26</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>27</v>
       </c>
@@ -4748,7 +4786,7 @@
         <v>1,2,3,4,13,14,15,16,25,26,27</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>28</v>
       </c>
@@ -4757,7 +4795,7 @@
         <v>1,2,3,4,13,14,15,16,25,26,27,28</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>37</v>
       </c>
@@ -4766,7 +4804,7 @@
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>38</v>
       </c>
@@ -4775,7 +4813,7 @@
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>39</v>
       </c>
@@ -4784,7 +4822,7 @@
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>40</v>
       </c>
@@ -4793,7 +4831,7 @@
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>49</v>
       </c>
@@ -4802,7 +4840,7 @@
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>50</v>
       </c>
@@ -4811,7 +4849,7 @@
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>51</v>
       </c>
@@ -4820,7 +4858,7 @@
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>52</v>
       </c>
@@ -4829,7 +4867,7 @@
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>61</v>
       </c>
@@ -4838,7 +4876,7 @@
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>62</v>
       </c>
@@ -4847,7 +4885,7 @@
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>63</v>
       </c>
@@ -4856,7 +4894,7 @@
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>64</v>
       </c>
@@ -4865,463 +4903,463 @@
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B25" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B26" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B27" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B28" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B29" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B30" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B31" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B32" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B33" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B34" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B35" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B36" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B37" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B38" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B39" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B40" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B41" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B42" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B43" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B44" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B45" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B46" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B47" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B48" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B49" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B50" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B51" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B52" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B53" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B54" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B55" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B56" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B57" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B58" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B59" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B60" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B61" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B62" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B63" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B64" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B65" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B66" t="str">
         <f t="shared" si="0"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B67" t="str">
         <f t="shared" ref="B67:B101" si="1">B66&amp;","&amp;A67</f>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B68" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B69" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B70" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B71" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B72" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B73" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B74" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B75" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B76" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B77" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B78" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B79" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B80" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B81" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B82" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B83" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B84" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B85" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B86" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B87" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B88" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B89" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B90" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B91" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B92" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B93" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B94" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B95" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B96" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B97" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B98" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B99" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B100" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B101" t="str">
         <f t="shared" si="1"/>
         <v>1,2,3,4,13,14,15,16,25,26,27,28,37,38,39,40,49,50,51,52,61,62,63,64,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,,</v>

</xml_diff>